<commit_message>
[GEN MAIN] Simulation update
</commit_message>
<xml_diff>
--- a/2_LF_Generator_Main/3_Review data/LF_Generator Main PCB review Data V1.0.xlsx
+++ b/2_LF_Generator_Main/3_Review data/LF_Generator Main PCB review Data V1.0.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Board dead 원인 파악</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -163,6 +163,38 @@
   </si>
   <si>
     <t>=&gt; Snubber가 없는 경우, Transformer의 전류가 안정화되지 않는다. Snubber 추가시 0.4msec내에 안정화 된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uH</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -510,6 +542,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,9 +566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
@@ -1542,10 +1574,10 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+      <c r="B9" s="21">
         <v>1</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
@@ -1556,8 +1588,8 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
       <c r="D10" t="s">
         <v>3</v>
       </c>
@@ -1566,28 +1598,28 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
       <c r="D11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="18">
+      <c r="B14" s="21">
         <v>2</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1598,8 +1630,8 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
       <c r="D15" t="s">
         <v>7</v>
       </c>
@@ -1608,8 +1640,8 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
       <c r="D16" t="s">
         <v>22</v>
       </c>
@@ -1618,8 +1650,8 @@
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1638,7 +1670,7 @@
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1649,8 +1681,8 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
@@ -1658,8 +1690,8 @@
         <v>14</v>
       </c>
       <c r="F2" s="9"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
       <c r="J2" s="10" t="s">
         <v>13</v>
       </c>
@@ -1669,10 +1701,10 @@
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="11">
         <v>1</v>
       </c>
@@ -1680,10 +1712,10 @@
         <v>5</v>
       </c>
       <c r="F3" s="17"/>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="22"/>
+      <c r="I3" s="25"/>
       <c r="J3" s="11">
         <v>1</v>
       </c>
@@ -1693,23 +1725,23 @@
       <c r="L3" s="17"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="12">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="E4" s="4">
         <f>D4*E3</f>
-        <v>1100</v>
+        <v>750</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -1727,7 +1759,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
@@ -1741,7 +1773,7 @@
       <c r="F5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="15" t="s">
         <v>10</v>
       </c>
@@ -1757,22 +1789,22 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="13">
         <f>D5/D4</f>
-        <v>1.3636363636363635</v>
+        <v>2</v>
       </c>
       <c r="E6" s="5">
         <f>E5/E4</f>
-        <v>0.27272727272727271</v>
+        <v>0.4</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1789,7 +1821,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1805,7 +1837,7 @@
       <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="26" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="15" t="s">
@@ -1823,7 +1855,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1869,7 @@
       <c r="F8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="15" t="s">
         <v>10</v>
       </c>
@@ -1853,7 +1885,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="16" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1900,7 @@
       <c r="F9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="24"/>
+      <c r="H9" s="27"/>
       <c r="I9" s="16" t="s">
         <v>12</v>
       </c>
@@ -1913,7 +1945,7 @@
   <dimension ref="B4:C119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:L3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1922,42 +1954,42 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="27" t="s">
+      <c r="C66" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C118" s="25" t="s">
+      <c r="C118" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C119" s="26" t="s">
+      <c r="C119" s="19" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1971,15 +2003,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E4"/>
+  <dimension ref="C3:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>25</v>
       </c>
@@ -1990,7 +2022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>28</v>
       </c>
@@ -1999,6 +2031,57 @@
       </c>
       <c r="E4" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7">
+        <v>600</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <f>D7*(G8/G7)</f>
+        <v>750</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8">
+        <f>D8^2*I7/(D7^2)</f>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GEN MAIN] Snubber review data update
</commit_message>
<xml_diff>
--- a/2_LF_Generator_Main/3_Review data/LF_Generator Main PCB review Data V1.0.xlsx
+++ b/2_LF_Generator_Main/3_Review data/LF_Generator Main PCB review Data V1.0.xlsx
@@ -1,107 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Power" sheetId="2" r:id="rId1"/>
     <sheet name="Transformer" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="Snubber Review" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
+    <sheet name="Snubber" sheetId="6" r:id="rId3"/>
+    <sheet name="Load Resistance" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
-  <si>
-    <t>Zener Diode Vz=10V Izsm=454mA 1W 5% DO-41</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1N4740A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Onsemi</t>
-  </si>
-  <si>
-    <t>Zener Diode Vz=15V Izsm=304mA 1W 5% DO-41</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1N4744A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1) Snubber 회로 추가시 Vgs 변화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Snubber 회로 검토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>=&gt; Pulse Off시 역으로 걸리는 전압이 떨어진다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2) Snubber 회로 추가시 전류 변화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>=&gt; FET의 전류가 삼각파 형태를 띄며, Low FET의 경우에는 전류 방향이 반대로 흐른다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>=&gt; FET의 전류가 구형파 형태를 띄며, Low FET도 정상 방향으로 흐른다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3) Snubber 회로 추가시 Transformer 전류 변화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>=&gt; Snubber가 없는 경우, Transformer의 전류가 안정화되지 않는다. Snubber 추가시 0.4msec내에 안정화 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>L1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>L2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>Inductance[uH]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -369,7 +285,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>I</t>
+    <t>Turn-off시 Peak Voltage 감소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ringring을 줄여줌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRFP460 I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -377,7 +301,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R</t>
+    <t>IRFP460 V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -385,15 +309,148 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Turn-off시 Peak Voltage 감소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ringring을 줄여줌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IRFP460C 의 Output Capacitance Cp= 460pF</t>
+    <t>Coss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ctotal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRFP460 P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pdiss_Rs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRFP460C 의 Output Capacitance Coss= 460pF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ω</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC Snubber Parameter calculation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N1/N2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load에 따른 MOSFET Current</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load resistance가 떨어지면 MOSFET에 흐르는 current가 상승하여 MOSFET에 damage가 발생함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MOSFET의 continuouse Drain current가 12.5A(Tc=100</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>℃)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>이므로 Load를 300Ω 이하로 떨어지지 않게 해야 한다.</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -404,9 +461,9 @@
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.000"/>
     <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.0\ &quot;%&quot;"/>
+    <numFmt numFmtId="178" formatCode="0.0\ &quot;%&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +504,21 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="5">
@@ -874,14 +946,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1006,10 +1077,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1025,7 +1093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1044,6 +1112,42 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1118,26 +1222,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2102,12 +2186,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="300435728"/>
-        <c:axId val="300523232"/>
+        <c:axId val="244093440"/>
+        <c:axId val="235695488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="300435728"/>
+        <c:axId val="244093440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2149,26 +2234,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ko-KR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2207,7 +2272,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300523232"/>
+        <c:crossAx val="235695488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2215,7 +2280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300523232"/>
+        <c:axId val="235695488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2271,26 +2336,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ko-KR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2323,7 +2368,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300435728"/>
+        <c:crossAx val="244093440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2964,14 +3009,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>684772</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>408547</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
@@ -3964,897 +4009,42 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>610635</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47822</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="그림 1"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="11144250" y="2371725"/>
-          <a:ext cx="7515225" cy="5448300"/>
+          <a:off x="952500" y="2847975"/>
+          <a:ext cx="7411485" cy="1409897"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1395254" cy="530658"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11706225" y="2657475"/>
-          <a:ext cx="1395254" cy="530658"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Red : </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Origin</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="ko-KR" sz="1400" b="1">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Green : Snubber</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14478000" y="2028825"/>
-          <a:ext cx="838200" cy="1790700"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="B7DEE8">
-            <a:alpha val="43922"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14658975" y="4648200"/>
-          <a:ext cx="838200" cy="1790700"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="B7DEE8">
-            <a:alpha val="43922"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="그림 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1162050" y="7419975"/>
-          <a:ext cx="13458825" cy="5524500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>16965</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="그림 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1123951" y="13763625"/>
-          <a:ext cx="6153150" cy="5112840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>125274</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>518578</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="그림 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7400924" y="13746024"/>
-          <a:ext cx="9243479" cy="3741876"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>183959</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="그림 12"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1152525" y="19621501"/>
-          <a:ext cx="6105525" cy="4870258"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>277511</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="그림 14"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7487936" y="19535776"/>
-          <a:ext cx="9771363" cy="4076700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>638176</xdr:colOff>
-      <xdr:row>158</xdr:row>
-      <xdr:rowOff>68714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="그림 16"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1143001" y="29051250"/>
-          <a:ext cx="11506200" cy="4545464"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>86051</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="그림 18"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6562725" y="24784050"/>
-          <a:ext cx="4333875" cy="4010351"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>681053</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="그림 20"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1171575" y="24803100"/>
-          <a:ext cx="4662503" cy="4038600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="그림 13"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1257300" y="781050"/>
-          <a:ext cx="7515225" cy="5448300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1395254" cy="530658"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="TextBox 15"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1819275" y="1066800"/>
-          <a:ext cx="1395254" cy="530658"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Red : </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Origin</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="ko-KR" sz="1400" b="1">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Green : Snubber</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4901,7 +4091,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4936,7 +4126,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5147,8 +4337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5166,7 +4356,7 @@
   <sheetData>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -5182,39 +4372,39 @@
     </row>
     <row r="4" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>68</v>
+      <c r="D5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>50</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>10</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <v>2</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="16">
         <v>82</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>50</v>
       </c>
       <c r="E7" s="2">
@@ -5223,569 +4413,661 @@
       <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <v>182</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>50</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>100</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>900</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="2:15" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>68</v>
+      <c r="D10" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>50</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>20</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <v>2</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="16">
         <v>182</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>30</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>20</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>3.2</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="3"/>
       <c r="D16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="39"/>
-      <c r="E17" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D18" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="49">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="38"/>
+      <c r="E17" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D18" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="48">
         <v>220</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="25">
         <v>220</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="25">
         <v>220</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="25">
         <v>220</v>
       </c>
-      <c r="I18" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D19" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="50">
+      <c r="I18" s="25">
+        <v>220</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="49">
         <v>300</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="28">
         <v>300</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="90">
         <f>G18*(2^0.5)</f>
         <v>311.12698372208092</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="27">
+        <v>300</v>
+      </c>
+      <c r="I19" s="28">
         <v>220</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D20" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="36">
+      <c r="J19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D20" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="35">
         <f>E19/2</f>
         <v>150</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="27">
         <f>F19/2</f>
         <v>150</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="27">
         <f>G19/2</f>
         <v>155.56349186104046</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="27">
+        <f>H19/2</f>
+        <v>150</v>
+      </c>
+      <c r="I20" s="28">
         <v>220</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D21" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="50">
+      <c r="J20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N20"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D21" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="49">
         <v>18.8</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="91">
         <v>18.8</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="91">
         <v>20</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="91">
         <v>12.5</v>
       </c>
-      <c r="I21" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D22" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="36">
+      <c r="I21" s="29">
+        <v>12.5</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D22" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="35">
         <f>E20*E21</f>
         <v>2820</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="27">
         <f>F20*F21</f>
         <v>2820</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="27">
         <f>G20*G21</f>
         <v>3111.2698372208092</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="27">
         <f>H20*H21</f>
+        <v>1875</v>
+      </c>
+      <c r="I22" s="27">
+        <f>I20*I21</f>
         <v>2750</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D23" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="50">
+      <c r="J22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="19"/>
+      <c r="N22"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="49">
         <v>5</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="28">
         <v>5</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="28">
         <v>5</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="28">
         <v>5</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D24" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="50">
+      <c r="I23" s="28">
+        <v>5</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D24" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="49">
         <v>720</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="27">
         <f>F20*F23</f>
         <v>750</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="27">
         <f>G20*G23</f>
         <v>777.81745930520231</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="27">
         <f>H20*H23</f>
+        <v>750</v>
+      </c>
+      <c r="I24" s="28">
+        <f>I20*I23</f>
         <v>1100</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D25" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="37">
+      <c r="J24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D25" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="36">
         <v>3.67</v>
       </c>
-      <c r="F25" s="31">
+      <c r="F25" s="30">
         <f>F22/F24</f>
         <v>3.76</v>
       </c>
-      <c r="G25" s="31">
+      <c r="G25" s="30">
         <f>G22/G24</f>
         <v>4</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="30">
         <f>H22/H24</f>
         <v>2.5</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D26" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="50">
+      <c r="I25" s="28">
+        <f>I22/I24</f>
+        <v>2.5</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D26" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="49">
         <v>10</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>10</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="28">
         <v>10</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="28">
         <v>10</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="M26" s="1"/>
-      <c r="N26"/>
-    </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D27" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="50">
+      <c r="I26" s="28">
+        <v>10</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D27" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="49">
         <f>E26*2</f>
         <v>20</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="28">
         <f>F26*2</f>
         <v>20</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="28">
         <f>G26*2</f>
         <v>20</v>
       </c>
-      <c r="H27" s="29">
+      <c r="H27" s="28">
         <f>H26*2</f>
         <v>20</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" t="s">
-        <v>55</v>
-      </c>
-      <c r="M27" s="1"/>
-      <c r="N27"/>
-    </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D28" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="50">
+      <c r="I27" s="28">
+        <f>I26*2</f>
+        <v>20</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D28" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="49">
         <f>E22*E27/100</f>
         <v>564</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="28">
         <f>F22*F27/100</f>
         <v>564</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="27">
         <f>G22*G27/100</f>
         <v>622.25396744416184</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="27">
         <f>H22*H27/100</f>
+        <v>375</v>
+      </c>
+      <c r="I28" s="28">
+        <f>I22*I27/100</f>
         <v>550</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D29" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="38">
+      <c r="J28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" t="s">
+        <v>57</v>
+      </c>
+      <c r="N28"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D29" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="37">
         <v>300</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="31">
         <v>300</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="31">
         <v>300</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="31">
         <v>300</v>
       </c>
-      <c r="I29" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D30" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="51">
+      <c r="I29" s="31">
+        <v>300</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D30" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="50">
         <f>E29/E28</f>
         <v>0.53191489361702127</v>
       </c>
-      <c r="F30" s="52">
+      <c r="F30" s="51">
         <f>F29/F28</f>
         <v>0.53191489361702127</v>
       </c>
-      <c r="G30" s="52">
+      <c r="G30" s="51">
         <f>G29/G28</f>
         <v>0.48211825989991874</v>
       </c>
-      <c r="H30" s="52">
+      <c r="H30" s="51">
         <f>H29/H28</f>
+        <v>0.8</v>
+      </c>
+      <c r="I30" s="51">
+        <f>I29/I28</f>
         <v>0.54545454545454541</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="4:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="53">
+      <c r="J30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K30" t="s">
+        <v>48</v>
+      </c>
+      <c r="N30"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="4:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="52">
         <f>E30*5</f>
         <v>2.6595744680851063</v>
       </c>
-      <c r="F31" s="54">
+      <c r="F31" s="53">
         <f>F30*5</f>
         <v>2.6595744680851063</v>
       </c>
-      <c r="G31" s="54">
+      <c r="G31" s="53">
         <f>G30*5</f>
         <v>2.4105912994995937</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="53">
         <f>H30*5</f>
+        <v>4</v>
+      </c>
+      <c r="I31" s="53">
+        <f>I30*5</f>
         <v>2.7272727272727271</v>
       </c>
-      <c r="I31" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D32" s="44" t="s">
+      <c r="J31" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="55">
+      <c r="N31"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D32" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="54">
         <v>50</v>
       </c>
-      <c r="F32" s="56">
+      <c r="F32" s="55">
         <v>50</v>
       </c>
-      <c r="G32" s="56">
+      <c r="G32" s="55">
         <v>50</v>
       </c>
-      <c r="H32" s="56">
+      <c r="H32" s="55">
         <v>50</v>
       </c>
-      <c r="I32" s="34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D33" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="50">
+      <c r="I32" s="55">
+        <v>50</v>
+      </c>
+      <c r="J32" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="N32"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D33" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="49">
         <f>1/E32</f>
         <v>0.02</v>
       </c>
-      <c r="F33" s="29">
+      <c r="F33" s="28">
         <f>1/F32</f>
         <v>0.02</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="28">
         <f>1/G32</f>
         <v>0.02</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="28">
         <f>1/H32</f>
         <v>0.02</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="57">
+      <c r="I33" s="28">
+        <f>1/I32</f>
+        <v>0.02</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N33"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="56">
         <f>E31/E33</f>
         <v>132.97872340425531</v>
       </c>
-      <c r="F34" s="58">
+      <c r="F34" s="57">
         <f>F31/F33</f>
         <v>132.97872340425531</v>
       </c>
-      <c r="G34" s="58">
+      <c r="G34" s="57">
         <f>G31/G33</f>
         <v>120.52956497497968</v>
       </c>
-      <c r="H34" s="58">
+      <c r="H34" s="57">
         <f>H31/H33</f>
+        <v>200</v>
+      </c>
+      <c r="I34" s="57">
+        <f>I31/I33</f>
         <v>136.36363636363635</v>
       </c>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C35" s="47"/>
-      <c r="D35" s="48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J34" s="8"/>
+      <c r="N34"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C35" s="46"/>
+      <c r="D35" s="47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D36" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C38" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D39" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="E39" s="73">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D39" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="71">
         <v>2820</v>
       </c>
-      <c r="F39" s="59">
+      <c r="F39" s="58">
         <v>2820</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D40" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="74">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D40" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="72">
         <v>10</v>
       </c>
-      <c r="F40" s="66">
+      <c r="F40" s="64">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D41" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" s="75">
+    <row r="41" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="73">
         <f>E39*E40*2/100</f>
         <v>564</v>
       </c>
-      <c r="F41" s="60">
+      <c r="F41" s="59">
         <f>F39*F40*2/100</f>
         <v>846</v>
       </c>
     </row>
-    <row r="42" spans="3:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="D42" s="70" t="s">
-        <v>76</v>
-      </c>
-      <c r="E42" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="G42" s="79" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D43" s="71">
+    <row r="42" spans="3:15" ht="33" x14ac:dyDescent="0.3">
+      <c r="D42" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="77" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D43" s="69">
         <v>20</v>
       </c>
-      <c r="E43" s="77">
+      <c r="E43" s="75">
         <f>($D43/E$41)*5</f>
         <v>0.1773049645390071</v>
       </c>
-      <c r="F43" s="62">
+      <c r="F43" s="61">
         <f>($D43/F$41)*5</f>
         <v>0.1182033096926714</v>
       </c>
@@ -5793,15 +5075,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D44" s="71">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D44" s="69">
         <v>40</v>
       </c>
-      <c r="E44" s="77">
+      <c r="E44" s="75">
         <f t="shared" ref="E44:F87" si="0">($D44/E$41)*5</f>
         <v>0.3546099290780142</v>
       </c>
-      <c r="F44" s="62">
+      <c r="F44" s="61">
         <f t="shared" si="0"/>
         <v>0.2364066193853428</v>
       </c>
@@ -5809,15 +5091,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D45" s="71">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D45" s="69">
         <v>60</v>
       </c>
-      <c r="E45" s="77">
+      <c r="E45" s="75">
         <f t="shared" si="0"/>
         <v>0.53191489361702127</v>
       </c>
-      <c r="F45" s="62">
+      <c r="F45" s="61">
         <f t="shared" si="0"/>
         <v>0.3546099290780142</v>
       </c>
@@ -5825,15 +5107,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D46" s="71">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D46" s="69">
         <v>80</v>
       </c>
-      <c r="E46" s="77">
+      <c r="E46" s="75">
         <f t="shared" si="0"/>
         <v>0.70921985815602839</v>
       </c>
-      <c r="F46" s="62">
+      <c r="F46" s="61">
         <f t="shared" si="0"/>
         <v>0.4728132387706856</v>
       </c>
@@ -5841,15 +5123,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D47" s="71">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D47" s="69">
         <v>100</v>
       </c>
-      <c r="E47" s="77">
+      <c r="E47" s="75">
         <f t="shared" si="0"/>
         <v>0.88652482269503552</v>
       </c>
-      <c r="F47" s="62">
+      <c r="F47" s="61">
         <f t="shared" si="0"/>
         <v>0.59101654846335694</v>
       </c>
@@ -5857,15 +5139,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D48" s="71">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D48" s="69">
         <v>120</v>
       </c>
-      <c r="E48" s="77">
+      <c r="E48" s="75">
         <f t="shared" si="0"/>
         <v>1.0638297872340425</v>
       </c>
-      <c r="F48" s="62">
+      <c r="F48" s="61">
         <f t="shared" si="0"/>
         <v>0.70921985815602839</v>
       </c>
@@ -5874,14 +5156,14 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D49" s="71">
+      <c r="D49" s="69">
         <v>140</v>
       </c>
-      <c r="E49" s="77">
+      <c r="E49" s="75">
         <f t="shared" si="0"/>
         <v>1.2411347517730495</v>
       </c>
-      <c r="F49" s="62">
+      <c r="F49" s="61">
         <f t="shared" si="0"/>
         <v>0.82742316784869974</v>
       </c>
@@ -5890,14 +5172,14 @@
       </c>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D50" s="71">
+      <c r="D50" s="69">
         <v>160</v>
       </c>
-      <c r="E50" s="77">
+      <c r="E50" s="75">
         <f t="shared" si="0"/>
         <v>1.4184397163120568</v>
       </c>
-      <c r="F50" s="62">
+      <c r="F50" s="61">
         <f t="shared" si="0"/>
         <v>0.94562647754137119</v>
       </c>
@@ -5906,14 +5188,14 @@
       </c>
     </row>
     <row r="51" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D51" s="71">
+      <c r="D51" s="69">
         <v>180</v>
       </c>
-      <c r="E51" s="77">
+      <c r="E51" s="75">
         <f t="shared" si="0"/>
         <v>1.5957446808510638</v>
       </c>
-      <c r="F51" s="62">
+      <c r="F51" s="61">
         <f t="shared" si="0"/>
         <v>1.0638297872340425</v>
       </c>
@@ -5922,14 +5204,14 @@
       </c>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D52" s="71">
+      <c r="D52" s="69">
         <v>200</v>
       </c>
-      <c r="E52" s="77">
+      <c r="E52" s="75">
         <f t="shared" si="0"/>
         <v>1.773049645390071</v>
       </c>
-      <c r="F52" s="62">
+      <c r="F52" s="61">
         <f t="shared" si="0"/>
         <v>1.1820330969267139</v>
       </c>
@@ -5938,14 +5220,14 @@
       </c>
     </row>
     <row r="53" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D53" s="71">
+      <c r="D53" s="69">
         <v>220</v>
       </c>
-      <c r="E53" s="77">
+      <c r="E53" s="75">
         <f t="shared" si="0"/>
         <v>1.9503546099290781</v>
       </c>
-      <c r="F53" s="62">
+      <c r="F53" s="61">
         <f t="shared" si="0"/>
         <v>1.3002364066193852</v>
       </c>
@@ -5954,14 +5236,14 @@
       </c>
     </row>
     <row r="54" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D54" s="71">
+      <c r="D54" s="69">
         <v>240</v>
       </c>
-      <c r="E54" s="77">
+      <c r="E54" s="75">
         <f t="shared" si="0"/>
         <v>2.1276595744680851</v>
       </c>
-      <c r="F54" s="62">
+      <c r="F54" s="61">
         <f t="shared" si="0"/>
         <v>1.4184397163120568</v>
       </c>
@@ -5970,14 +5252,14 @@
       </c>
     </row>
     <row r="55" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D55" s="71">
+      <c r="D55" s="69">
         <v>260</v>
       </c>
-      <c r="E55" s="77">
+      <c r="E55" s="75">
         <f t="shared" si="0"/>
         <v>2.3049645390070923</v>
       </c>
-      <c r="F55" s="62">
+      <c r="F55" s="61">
         <f t="shared" si="0"/>
         <v>1.5366430260047281</v>
       </c>
@@ -5986,14 +5268,14 @@
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D56" s="71">
+      <c r="D56" s="69">
         <v>280</v>
       </c>
-      <c r="E56" s="77">
+      <c r="E56" s="75">
         <f t="shared" si="0"/>
         <v>2.4822695035460991</v>
       </c>
-      <c r="F56" s="62">
+      <c r="F56" s="61">
         <f t="shared" si="0"/>
         <v>1.6548463356973995</v>
       </c>
@@ -6002,14 +5284,14 @@
       </c>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D57" s="71">
+      <c r="D57" s="69">
         <v>300</v>
       </c>
-      <c r="E57" s="77">
+      <c r="E57" s="75">
         <f t="shared" si="0"/>
         <v>2.6595744680851063</v>
       </c>
-      <c r="F57" s="62">
+      <c r="F57" s="61">
         <f t="shared" si="0"/>
         <v>1.773049645390071</v>
       </c>
@@ -6018,14 +5300,14 @@
       </c>
     </row>
     <row r="58" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D58" s="71">
+      <c r="D58" s="69">
         <v>320</v>
       </c>
-      <c r="E58" s="77">
+      <c r="E58" s="75">
         <f t="shared" si="0"/>
         <v>2.8368794326241136</v>
       </c>
-      <c r="F58" s="62">
+      <c r="F58" s="61">
         <f t="shared" si="0"/>
         <v>1.8912529550827424</v>
       </c>
@@ -6034,14 +5316,14 @@
       </c>
     </row>
     <row r="59" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D59" s="71">
+      <c r="D59" s="69">
         <v>340</v>
       </c>
-      <c r="E59" s="77">
+      <c r="E59" s="75">
         <f t="shared" si="0"/>
         <v>3.0141843971631204</v>
       </c>
-      <c r="F59" s="62">
+      <c r="F59" s="61">
         <f t="shared" si="0"/>
         <v>2.0094562647754137</v>
       </c>
@@ -6050,14 +5332,14 @@
       </c>
     </row>
     <row r="60" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D60" s="71">
+      <c r="D60" s="69">
         <v>360</v>
       </c>
-      <c r="E60" s="77">
+      <c r="E60" s="75">
         <f t="shared" si="0"/>
         <v>3.1914893617021276</v>
       </c>
-      <c r="F60" s="62">
+      <c r="F60" s="61">
         <f t="shared" si="0"/>
         <v>2.1276595744680851</v>
       </c>
@@ -6066,14 +5348,14 @@
       </c>
     </row>
     <row r="61" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D61" s="71">
+      <c r="D61" s="69">
         <v>380</v>
       </c>
-      <c r="E61" s="77">
+      <c r="E61" s="75">
         <f t="shared" si="0"/>
         <v>3.3687943262411348</v>
       </c>
-      <c r="F61" s="62">
+      <c r="F61" s="61">
         <f t="shared" si="0"/>
         <v>2.2458628841607564</v>
       </c>
@@ -6082,14 +5364,14 @@
       </c>
     </row>
     <row r="62" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D62" s="71">
+      <c r="D62" s="69">
         <v>400</v>
       </c>
-      <c r="E62" s="77">
+      <c r="E62" s="75">
         <f t="shared" si="0"/>
         <v>3.5460992907801421</v>
       </c>
-      <c r="F62" s="62">
+      <c r="F62" s="61">
         <f t="shared" si="0"/>
         <v>2.3640661938534278</v>
       </c>
@@ -6098,14 +5380,14 @@
       </c>
     </row>
     <row r="63" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D63" s="71">
+      <c r="D63" s="69">
         <v>420</v>
       </c>
-      <c r="E63" s="77">
+      <c r="E63" s="75">
         <f t="shared" si="0"/>
         <v>3.7234042553191489</v>
       </c>
-      <c r="F63" s="62">
+      <c r="F63" s="61">
         <f t="shared" si="0"/>
         <v>2.4822695035460991</v>
       </c>
@@ -6114,14 +5396,14 @@
       </c>
     </row>
     <row r="64" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D64" s="71">
+      <c r="D64" s="69">
         <v>440</v>
       </c>
-      <c r="E64" s="77">
+      <c r="E64" s="75">
         <f t="shared" si="0"/>
         <v>3.9007092198581561</v>
       </c>
-      <c r="F64" s="62">
+      <c r="F64" s="61">
         <f t="shared" si="0"/>
         <v>2.6004728132387704</v>
       </c>
@@ -6130,14 +5412,14 @@
       </c>
     </row>
     <row r="65" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D65" s="71">
+      <c r="D65" s="69">
         <v>460</v>
       </c>
-      <c r="E65" s="77">
+      <c r="E65" s="75">
         <f t="shared" si="0"/>
         <v>4.0780141843971629</v>
       </c>
-      <c r="F65" s="62">
+      <c r="F65" s="61">
         <f t="shared" si="0"/>
         <v>2.7186761229314422</v>
       </c>
@@ -6146,14 +5428,14 @@
       </c>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D66" s="71">
+      <c r="D66" s="69">
         <v>480</v>
       </c>
-      <c r="E66" s="77">
+      <c r="E66" s="75">
         <f t="shared" si="0"/>
         <v>4.2553191489361701</v>
       </c>
-      <c r="F66" s="62">
+      <c r="F66" s="61">
         <f t="shared" si="0"/>
         <v>2.8368794326241136</v>
       </c>
@@ -6162,14 +5444,14 @@
       </c>
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D67" s="71">
+      <c r="D67" s="69">
         <v>500</v>
       </c>
-      <c r="E67" s="77">
+      <c r="E67" s="75">
         <f t="shared" si="0"/>
         <v>4.4326241134751774</v>
       </c>
-      <c r="F67" s="62">
+      <c r="F67" s="61">
         <f t="shared" si="0"/>
         <v>2.9550827423167849</v>
       </c>
@@ -6178,14 +5460,14 @@
       </c>
     </row>
     <row r="68" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D68" s="71">
+      <c r="D68" s="69">
         <v>520</v>
       </c>
-      <c r="E68" s="77">
+      <c r="E68" s="75">
         <f t="shared" si="0"/>
         <v>4.6099290780141846</v>
       </c>
-      <c r="F68" s="62">
+      <c r="F68" s="61">
         <f t="shared" si="0"/>
         <v>3.0732860520094563</v>
       </c>
@@ -6194,14 +5476,14 @@
       </c>
     </row>
     <row r="69" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D69" s="71">
+      <c r="D69" s="69">
         <v>540</v>
       </c>
-      <c r="E69" s="77">
+      <c r="E69" s="75">
         <f t="shared" si="0"/>
         <v>4.7872340425531918</v>
       </c>
-      <c r="F69" s="62">
+      <c r="F69" s="61">
         <f t="shared" si="0"/>
         <v>3.1914893617021276</v>
       </c>
@@ -6210,14 +5492,14 @@
       </c>
     </row>
     <row r="70" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D70" s="71">
+      <c r="D70" s="69">
         <v>560</v>
       </c>
-      <c r="E70" s="77">
+      <c r="E70" s="75">
         <f t="shared" si="0"/>
         <v>4.9645390070921982</v>
       </c>
-      <c r="F70" s="62">
+      <c r="F70" s="61">
         <f t="shared" si="0"/>
         <v>3.3096926713947989</v>
       </c>
@@ -6226,14 +5508,14 @@
       </c>
     </row>
     <row r="71" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D71" s="71">
+      <c r="D71" s="69">
         <v>580</v>
       </c>
-      <c r="E71" s="77">
+      <c r="E71" s="75">
         <f t="shared" si="0"/>
         <v>5.1418439716312054</v>
       </c>
-      <c r="F71" s="62">
+      <c r="F71" s="61">
         <f t="shared" si="0"/>
         <v>3.4278959810874703</v>
       </c>
@@ -6242,14 +5524,14 @@
       </c>
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D72" s="71">
+      <c r="D72" s="69">
         <v>600</v>
       </c>
-      <c r="E72" s="77">
+      <c r="E72" s="75">
         <f t="shared" si="0"/>
         <v>5.3191489361702127</v>
       </c>
-      <c r="F72" s="62">
+      <c r="F72" s="61">
         <f t="shared" si="0"/>
         <v>3.5460992907801421</v>
       </c>
@@ -6258,14 +5540,14 @@
       </c>
     </row>
     <row r="73" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D73" s="71">
+      <c r="D73" s="69">
         <v>620</v>
       </c>
-      <c r="E73" s="77">
+      <c r="E73" s="75">
         <f t="shared" si="0"/>
         <v>5.4964539007092199</v>
       </c>
-      <c r="F73" s="62">
+      <c r="F73" s="61">
         <f t="shared" si="0"/>
         <v>3.664302600472813</v>
       </c>
@@ -6274,14 +5556,14 @@
       </c>
     </row>
     <row r="74" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D74" s="71">
+      <c r="D74" s="69">
         <v>640</v>
       </c>
-      <c r="E74" s="77">
+      <c r="E74" s="75">
         <f t="shared" si="0"/>
         <v>5.6737588652482271</v>
       </c>
-      <c r="F74" s="62">
+      <c r="F74" s="61">
         <f t="shared" si="0"/>
         <v>3.7825059101654848</v>
       </c>
@@ -6290,14 +5572,14 @@
       </c>
     </row>
     <row r="75" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D75" s="71">
+      <c r="D75" s="69">
         <v>660</v>
       </c>
-      <c r="E75" s="77">
+      <c r="E75" s="75">
         <f t="shared" si="0"/>
         <v>5.8510638297872344</v>
       </c>
-      <c r="F75" s="62">
+      <c r="F75" s="61">
         <f t="shared" si="0"/>
         <v>3.9007092198581561</v>
       </c>
@@ -6306,14 +5588,14 @@
       </c>
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D76" s="71">
+      <c r="D76" s="69">
         <v>680</v>
       </c>
-      <c r="E76" s="77">
+      <c r="E76" s="75">
         <f t="shared" si="0"/>
         <v>6.0283687943262407</v>
       </c>
-      <c r="F76" s="62">
+      <c r="F76" s="61">
         <f t="shared" si="0"/>
         <v>4.0189125295508275</v>
       </c>
@@ -6322,14 +5604,14 @@
       </c>
     </row>
     <row r="77" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D77" s="71">
+      <c r="D77" s="69">
         <v>700</v>
       </c>
-      <c r="E77" s="77">
+      <c r="E77" s="75">
         <f t="shared" si="0"/>
         <v>6.205673758865248</v>
       </c>
-      <c r="F77" s="62">
+      <c r="F77" s="61">
         <f t="shared" si="0"/>
         <v>4.1371158392434983</v>
       </c>
@@ -6338,14 +5620,14 @@
       </c>
     </row>
     <row r="78" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D78" s="71">
+      <c r="D78" s="69">
         <v>720</v>
       </c>
-      <c r="E78" s="77">
+      <c r="E78" s="75">
         <f t="shared" si="0"/>
         <v>6.3829787234042552</v>
       </c>
-      <c r="F78" s="62">
+      <c r="F78" s="61">
         <f t="shared" si="0"/>
         <v>4.2553191489361701</v>
       </c>
@@ -6354,14 +5636,14 @@
       </c>
     </row>
     <row r="79" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D79" s="71">
+      <c r="D79" s="69">
         <v>740</v>
       </c>
-      <c r="E79" s="77">
+      <c r="E79" s="75">
         <f t="shared" si="0"/>
         <v>6.5602836879432624</v>
       </c>
-      <c r="F79" s="62">
+      <c r="F79" s="61">
         <f t="shared" si="0"/>
         <v>4.3735224586288419</v>
       </c>
@@ -6370,14 +5652,14 @@
       </c>
     </row>
     <row r="80" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D80" s="71">
+      <c r="D80" s="69">
         <v>760</v>
       </c>
-      <c r="E80" s="77">
+      <c r="E80" s="75">
         <f t="shared" si="0"/>
         <v>6.7375886524822697</v>
       </c>
-      <c r="F80" s="62">
+      <c r="F80" s="61">
         <f t="shared" si="0"/>
         <v>4.4917257683215128</v>
       </c>
@@ -6386,14 +5668,14 @@
       </c>
     </row>
     <row r="81" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D81" s="71">
+      <c r="D81" s="69">
         <v>780</v>
       </c>
-      <c r="E81" s="77">
+      <c r="E81" s="75">
         <f t="shared" si="0"/>
         <v>6.9148936170212769</v>
       </c>
-      <c r="F81" s="62">
+      <c r="F81" s="61">
         <f t="shared" si="0"/>
         <v>4.6099290780141846</v>
       </c>
@@ -6402,14 +5684,14 @@
       </c>
     </row>
     <row r="82" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D82" s="71">
+      <c r="D82" s="69">
         <v>800</v>
       </c>
-      <c r="E82" s="77">
+      <c r="E82" s="75">
         <f t="shared" si="0"/>
         <v>7.0921985815602842</v>
       </c>
-      <c r="F82" s="62">
+      <c r="F82" s="61">
         <f t="shared" si="0"/>
         <v>4.7281323877068555</v>
       </c>
@@ -6418,14 +5700,14 @@
       </c>
     </row>
     <row r="83" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D83" s="71">
+      <c r="D83" s="69">
         <v>820</v>
       </c>
-      <c r="E83" s="77">
+      <c r="E83" s="75">
         <f t="shared" si="0"/>
         <v>7.2695035460992905</v>
       </c>
-      <c r="F83" s="62">
+      <c r="F83" s="61">
         <f t="shared" si="0"/>
         <v>4.8463356973995273</v>
       </c>
@@ -6434,14 +5716,14 @@
       </c>
     </row>
     <row r="84" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D84" s="71">
+      <c r="D84" s="69">
         <v>840</v>
       </c>
-      <c r="E84" s="77">
+      <c r="E84" s="75">
         <f t="shared" si="0"/>
         <v>7.4468085106382977</v>
       </c>
-      <c r="F84" s="62">
+      <c r="F84" s="61">
         <f t="shared" si="0"/>
         <v>4.9645390070921982</v>
       </c>
@@ -6450,14 +5732,14 @@
       </c>
     </row>
     <row r="85" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D85" s="71">
+      <c r="D85" s="69">
         <v>860</v>
       </c>
-      <c r="E85" s="77">
+      <c r="E85" s="75">
         <f t="shared" si="0"/>
         <v>7.624113475177305</v>
       </c>
-      <c r="F85" s="62">
+      <c r="F85" s="61">
         <f t="shared" si="0"/>
         <v>5.08274231678487</v>
       </c>
@@ -6466,14 +5748,14 @@
       </c>
     </row>
     <row r="86" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D86" s="71">
+      <c r="D86" s="69">
         <v>880</v>
       </c>
-      <c r="E86" s="77">
+      <c r="E86" s="75">
         <f t="shared" si="0"/>
         <v>7.8014184397163122</v>
       </c>
-      <c r="F86" s="62">
+      <c r="F86" s="61">
         <f t="shared" si="0"/>
         <v>5.2009456264775409</v>
       </c>
@@ -6482,14 +5764,14 @@
       </c>
     </row>
     <row r="87" spans="4:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D87" s="72">
+      <c r="D87" s="70">
         <v>900</v>
       </c>
-      <c r="E87" s="78">
+      <c r="E87" s="76">
         <f t="shared" si="0"/>
         <v>7.9787234042553195</v>
       </c>
-      <c r="F87" s="63">
+      <c r="F87" s="62">
         <f t="shared" si="0"/>
         <v>5.3191489361702127</v>
       </c>
@@ -6509,7 +5791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -6524,7 +5806,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -6534,99 +5816,99 @@
     </row>
     <row r="4" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D5" s="64" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="65"/>
+      <c r="D5" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="80"/>
     </row>
     <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>25</v>
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>100</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>983</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>100</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>24.19</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>10</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>597</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>10</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>14.96</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>594</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>1</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>14.96</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>0.12</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>594</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>0.12</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>15.03</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
-        <v>29</v>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="C12" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6642,127 +5924,482 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="4.75" customWidth="1"/>
+    <col min="1" max="2" width="4.75" customWidth="1"/>
+    <col min="3" max="3" width="4.875" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="15">
         <v>20</v>
       </c>
-      <c r="F10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12">
-        <f>E10*E11</f>
-        <v>12400</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
+      <c r="F8" s="15">
+        <v>20</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D9" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="2">
+        <v>150</v>
+      </c>
+      <c r="F9" s="2">
+        <v>150</v>
+      </c>
+      <c r="G9" s="82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D10" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="2">
+        <f>E8*E9</f>
+        <v>3000</v>
+      </c>
+      <c r="F10" s="2">
+        <f>F8*F9</f>
+        <v>3000</v>
+      </c>
+      <c r="G10" s="82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D11" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="2">
+        <v>460</v>
+      </c>
+      <c r="F11" s="2">
+        <v>460</v>
+      </c>
+      <c r="G11" s="82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D12" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="2">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2">
+        <v>40</v>
+      </c>
+      <c r="G12" s="82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="2">
+        <f>E11+E12</f>
+        <v>500</v>
+      </c>
+      <c r="F13" s="2">
+        <f>F11+F12</f>
+        <v>500</v>
+      </c>
+      <c r="G13" s="82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="2">
+        <f>E13*2</f>
+        <v>1000</v>
+      </c>
+      <c r="F14" s="2">
+        <f>F13*2</f>
+        <v>1000</v>
+      </c>
+      <c r="G14" s="82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="2">
+        <f>E9/E8</f>
+        <v>7.5</v>
+      </c>
+      <c r="F15" s="2">
+        <f>F9/F8</f>
+        <v>7.5</v>
+      </c>
+      <c r="G15" s="83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2">
+        <v>100</v>
+      </c>
+      <c r="F16" s="2">
+        <v>50</v>
+      </c>
+      <c r="G16" s="82" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="13">
+        <f>E14*(E9^2)*E16/10^9</f>
+        <v>2.25</v>
+      </c>
+      <c r="F17" s="13">
+        <f>F14*(F9^2)*F16/10^9</f>
+        <v>1.125</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C116"/>
+  <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
+    <col min="1" max="2" width="5" customWidth="1"/>
+    <col min="3" max="4" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="15">
+        <v>10</v>
+      </c>
+      <c r="E4" s="15">
+        <v>50</v>
+      </c>
+      <c r="F4" s="15">
+        <v>100</v>
+      </c>
+      <c r="G4" s="15">
+        <v>150</v>
+      </c>
+      <c r="H4" s="15">
+        <v>200</v>
+      </c>
+      <c r="I4" s="15">
+        <v>250</v>
+      </c>
+      <c r="J4" s="15">
+        <v>300</v>
+      </c>
+      <c r="K4" s="87" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="2">
+        <v>750</v>
+      </c>
+      <c r="E5" s="2">
+        <v>750</v>
+      </c>
+      <c r="F5" s="2">
+        <v>750</v>
+      </c>
+      <c r="G5" s="2">
+        <v>750</v>
+      </c>
+      <c r="H5" s="2">
+        <v>750</v>
+      </c>
+      <c r="I5" s="2">
+        <v>750</v>
+      </c>
+      <c r="J5" s="2">
+        <v>750</v>
+      </c>
+      <c r="K5" s="82" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="2">
+        <f>D5/D4</f>
+        <v>75</v>
+      </c>
+      <c r="E6" s="2">
+        <f>E5/E4</f>
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
+        <f>F5/F4</f>
+        <v>7.5</v>
+      </c>
+      <c r="G6" s="2">
+        <f>G5/G4</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C62" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C63" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C90" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C115" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C116" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="H6" s="2">
+        <f>H5/H4</f>
+        <v>3.75</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I5/I4</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <f>J5/J4</f>
+        <v>2.5</v>
+      </c>
+      <c r="K6" s="82" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="2">
+        <f>D6*D5</f>
+        <v>56250</v>
+      </c>
+      <c r="E7" s="2">
+        <f>E6*E5</f>
+        <v>11250</v>
+      </c>
+      <c r="F7" s="2">
+        <f>F6*F5</f>
+        <v>5625</v>
+      </c>
+      <c r="G7" s="2">
+        <f>G6*G5</f>
+        <v>3750</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H6*H5</f>
+        <v>2812.5</v>
+      </c>
+      <c r="I7" s="2">
+        <f>I6*I5</f>
+        <v>2250</v>
+      </c>
+      <c r="J7" s="2">
+        <f>J6*J5</f>
+        <v>1875</v>
+      </c>
+      <c r="K7" s="82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="82" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="2">
+        <f>D5/D8</f>
+        <v>150</v>
+      </c>
+      <c r="E9" s="2">
+        <f>E5/E8</f>
+        <v>150</v>
+      </c>
+      <c r="F9" s="2">
+        <f>F5/F8</f>
+        <v>150</v>
+      </c>
+      <c r="G9" s="2">
+        <f>G5/G8</f>
+        <v>150</v>
+      </c>
+      <c r="H9" s="2">
+        <f>H5/H8</f>
+        <v>150</v>
+      </c>
+      <c r="I9" s="2">
+        <f>I5/I8</f>
+        <v>150</v>
+      </c>
+      <c r="J9" s="2">
+        <f>J5/J8</f>
+        <v>150</v>
+      </c>
+      <c r="K9" s="82" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="13">
+        <f>D7/D9</f>
+        <v>375</v>
+      </c>
+      <c r="E10" s="13">
+        <f>E7/E9</f>
+        <v>75</v>
+      </c>
+      <c r="F10" s="13">
+        <f>F7/F9</f>
+        <v>37.5</v>
+      </c>
+      <c r="G10" s="13">
+        <f>G7/G9</f>
+        <v>25</v>
+      </c>
+      <c r="H10" s="13">
+        <f>H7/H9</f>
+        <v>18.75</v>
+      </c>
+      <c r="I10" s="13">
+        <f>I7/I9</f>
+        <v>15</v>
+      </c>
+      <c r="J10" s="13">
+        <f>J7/J9</f>
+        <v>12.5</v>
+      </c>
+      <c r="K10" s="59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="46"/>
+      <c r="C11" s="92" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="46"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="46"/>
+      <c r="C12" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6770,94 +6407,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>150</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7">
-        <v>600</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8">
-        <f>D7*(G8/G7)</f>
-        <v>750</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8">
-        <f>D8^2*I7/(D7^2)</f>
-        <v>15000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>